<commit_message>
Update Funtions and Global Variables.xlsx
</commit_message>
<xml_diff>
--- a/Funtions and Global Variables.xlsx
+++ b/Funtions and Global Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\최준영\학교\과제, 실습\2학년 2학기 (2019)\시스템 프로그래밍(홍석인)\Team Project\SP_2019_2_team1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559C1E3D-7087-4E50-85A3-0093E83499EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCC88B2-4EF8-423C-808A-76BF11BDA959}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C94E521-1522-41C2-B745-21FA71AF459A}"/>
   </bookViews>
@@ -34,23 +34,23 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="111">
   <si>
     <t>Function Usage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Arguments</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Returns</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>void *send_msg(void *)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Send message to server</t>
@@ -58,7 +58,7 @@
   <si>
     <t>0 if entered ‘q’ or ‘Q’
 NULL if success</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>void *recv_msg(void *)</t>
@@ -73,23 +73,23 @@
     <t>1 if read failed
 0 if entered ‘q’ or ‘Q’
 NULL if success</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>void *arg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>client.c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Global Variable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Initialize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>name[BUFSIZ]</t>
@@ -108,7 +108,7 @@
   </si>
   <si>
     <t>server.c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Client *addClient(int, char *)</t>
@@ -136,7 +136,7 @@
   </si>
   <si>
     <t>Room *addRoom(char *)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>void removeRoom(int)</t>
@@ -161,22 +161,22 @@
   </si>
   <si>
     <t>void printWaitingRoomMenu(Client *)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>void printRoomMenu(Client *)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>void printHowToUse(Client *)</t>
   </si>
   <si>
     <t>void serveWaitingRoomMenu(int, Client *, char *)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>void exitRoom(Client *)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>void serveRoomMenu(char *, Client *, char *)</t>
@@ -189,7 +189,7 @@
   </si>
   <si>
     <t>error 처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>빈 방인지 확인</t>
@@ -208,57 +208,57 @@
   </si>
   <si>
     <t>채팅방에서 사용할 수 있는 메뉴 보여줌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>대기화면에서 사용할 수 있는 메뉴 보여줌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>해당 채팅방에 있는 모든 client 나열</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>채팅방의 id를 얻어옴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>client에게 채팅방 목록 제공</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>room(채팅방) 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>client가 해당 채팅방에 입장</t>
   </si>
   <si>
     <t>특정 room(채팅방)이 존재하는지 확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>room_arr에서 room(채팅방) 삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>room_arr에 room(채팅방) 추가</t>
   </si>
   <si>
     <t>채팅방에서 client가 고른 menu 받아옴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>대기화면에서 client가 고른 menu 받아옴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>문자열에서 공백 확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>해당 client가 방에 있는지 체크</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>방의 모든 사용자에게 message 보냄</t>
@@ -268,7 +268,7 @@
   </si>
   <si>
     <t>client_arr에서 client 삭제(client disconnected)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>client_arr에 client 추가</t>
@@ -293,7 +293,7 @@
   </si>
   <si>
     <t>char *name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>int roomId</t>
@@ -306,11 +306,11 @@
   </si>
   <si>
     <t>Client *client</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>int socket</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>int menu, Client *client, char *msg</t>
@@ -320,7 +320,7 @@
   </si>
   <si>
     <t>int roomId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>void *handle_serv(void *)</t>
@@ -330,7 +330,7 @@
   </si>
   <si>
     <t>server 동작 제어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>client 동작 제어</t>
@@ -338,52 +338,52 @@
   <si>
     <t>0 if entered 'q' or 'Q'
 NULL if success</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>client</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>TRUE if client is in room
 FALSE if client is not in room</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>-1 if fail
 indexSpace (공백문자의 위치)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>0 if fail
 firstByte (사용자가 선택한 메뉴의 int형)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>return if fail or wrong message</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>room (생성된 방 구조체 변수의 주소)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>TRUE if room exists
 FALSE if room does not exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>roomId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>TRUE if empty
 FALSE if not empty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>NULL if success</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>pthread_mutex_t lock</t>
@@ -393,7 +393,7 @@
   </si>
   <si>
     <t>int client_size</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>접속중인 사용자 수(client_arr 배열의 size)</t>
@@ -409,7 +409,7 @@
   </si>
   <si>
     <t>room_arr 배열의 size</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Room room_arr[MAX_ROOM]</t>
@@ -428,7 +428,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,12 +478,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -487,44 +501,51 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - 강조색6" xfId="1" builtinId="50"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -839,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D47F9D4-56CF-4522-84D7-09FCFCB3F381}">
   <dimension ref="A3:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -950,7 +971,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="10" t="s">
         <v>84</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -971,7 +992,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1259,7 +1280,7 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+      <c r="B30" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C30" t="s">
@@ -1281,7 +1302,7 @@
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+      <c r="B32" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C32" t="s">
@@ -1317,7 +1338,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>

</xml_diff>